<commit_message>
Revisão Geral no Scrum
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Product Backlog - EveRemind.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Product Backlog - EveRemind.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr hidePivotFieldList="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="25808"/>
+  <workbookPr hidePivotFieldList="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciuscmac/Desktop/GitHub/P.I.-ES-UFG-2015-BIJLMMV/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="783"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="24220" windowHeight="16100" tabRatio="783"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -12,14 +17,19 @@
   <definedNames>
     <definedName name="AgendaAno">#REF!</definedName>
     <definedName name="AgendaSemestre">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Product Backlog'!$B$5:$G$12</definedName>
     <definedName name="Área_Impressão_Agenda">OFFSET(#REF!,,,COUNTA(#REF!))</definedName>
     <definedName name="Área_Impressão_Atribuição">OFFSET(#REF!,,,COUNTA(#REF!))</definedName>
     <definedName name="IníciodoCronograma">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Product Backlog'!$B$5:$G$12</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Product Backlog'!$4:$4</definedName>
     <definedName name="TérminoAgenda">#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Product Backlog'!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -148,8 +158,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -228,7 +238,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -272,10 +282,16 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -735,6 +751,11 @@
       <tableStyleElement type="firstColumn" dxfId="8"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -762,8 +783,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="114300" y="781050"/>
-          <a:ext cx="2162175" cy="514350"/>
+          <a:off x="114300" y="777875"/>
+          <a:ext cx="2108200" cy="514350"/>
           <a:chOff x="114300" y="781050"/>
           <a:chExt cx="1836964" cy="514350"/>
         </a:xfrm>
@@ -801,7 +822,7 @@
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
           <xdr:cNvPr id="1037" name="Lista de Aulas" descr="&quot;&quot;">
-            <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" invalidUrl="Estórias de usuário - Projeto EveRemind.docx"/>
           </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1"/>
@@ -1181,33 +1202,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="-0.499984740745262"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="68.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="82.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="74.3984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="82.796875" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="17.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.19921875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="50.25" customHeight="1">
+    <row r="1" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
         <v>6</v>
@@ -1218,7 +1239,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:10" ht="39" customHeight="1">
+    <row r="2" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1227,7 +1248,7 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="24.75" customHeight="1">
+    <row r="3" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1236,7 +1257,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="18" customHeight="1">
+    <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>1</v>
@@ -1257,7 +1278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18" customHeight="1">
+    <row r="5" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="10" t="s">
         <v>7</v>
@@ -1268,16 +1289,16 @@
       <c r="D5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="15" t="s">
         <v>26</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1">
+    <row r="6" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="12" t="s">
         <v>8</v>
@@ -1291,13 +1312,13 @@
       <c r="E6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="15" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1">
+    <row r="7" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="12" t="s">
         <v>9</v>
@@ -1311,13 +1332,13 @@
       <c r="E7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="15" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="18" customHeight="1">
+    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="12" t="s">
         <v>10</v>
@@ -1331,13 +1352,13 @@
       <c r="E8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="15" t="s">
         <v>29</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="18" customHeight="1">
+    <row r="9" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>11</v>
@@ -1351,13 +1372,13 @@
       <c r="E9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="15" t="s">
         <v>30</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="18" customHeight="1">
+    <row r="10" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="12" t="s">
         <v>12</v>
@@ -1371,13 +1392,13 @@
       <c r="E10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="18" customHeight="1">
+    <row r="11" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="12" t="s">
         <v>13</v>
@@ -1391,7 +1412,7 @@
       <c r="E11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="15" t="s">
         <v>32</v>
       </c>
       <c r="G11" s="12" t="s">
@@ -1399,7 +1420,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="18" customHeight="1">
+    <row r="12" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="13" t="s">
         <v>14</v>
@@ -1413,7 +1434,7 @@
       <c r="E12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="16" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="13"/>
@@ -1421,7 +1442,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="18" customHeight="1">
+    <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -1431,7 +1452,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="18" customHeight="1">
+    <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -1441,7 +1462,7 @@
       <c r="G14" s="14"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="18" customHeight="1">
+    <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -1451,7 +1472,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="18" customHeight="1">
+    <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H16" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[GPR] Atualizando o Método de Estimativa e o Orçamento no Plano de Projeto
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Product Backlog - EveRemind.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Product Backlog - EveRemind.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="25808"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr hidePivotFieldList="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciuscmac/Desktop/GitHub/P.I.-ES-UFG-2015-BIJLMMV/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Dropbox\Repositórios\GitHub\P.I.-ES-UFG-2015-BIJLMMV\Artefatos de Documentação\Processo Aplicado\EveRemind\2-Gerencia de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="24220" windowHeight="16100" tabRatio="783"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="24225" windowHeight="16095" tabRatio="783"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>NOME</t>
   </si>
@@ -108,14 +108,7 @@
     <t>Visualizar Atividade</t>
   </si>
   <si>
-    <t xml:space="preserve">9 pontos
-</t>
-  </si>
-  <si>
     <t>6 pontos</t>
-  </si>
-  <si>
-    <t>9 pontos</t>
   </si>
   <si>
     <t xml:space="preserve">Uma mensagem de cadastro bem sucedido é exibida.
@@ -153,13 +146,26 @@
   </si>
   <si>
     <t>Alta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 pontos
+</t>
+  </si>
+  <si>
+    <t>3 pontos</t>
+  </si>
+  <si>
+    <t>5 pontos</t>
+  </si>
+  <si>
+    <t>4 pontos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -755,6 +761,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -783,8 +792,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="114300" y="777875"/>
-          <a:ext cx="2108200" cy="514350"/>
+          <a:off x="123825" y="781050"/>
+          <a:ext cx="2162175" cy="514350"/>
           <a:chOff x="114300" y="781050"/>
           <a:chExt cx="1836964" cy="514350"/>
         </a:xfrm>
@@ -1203,32 +1212,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.19921875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="74.3984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="82.796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="74.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="82.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.19921875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="50.25" customHeight="1">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
         <v>6</v>
@@ -1239,7 +1248,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="39" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1248,7 +1257,7 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="24.75" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1257,7 +1266,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="18" customHeight="1">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>1</v>
@@ -1278,7 +1287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="36" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="10" t="s">
         <v>7</v>
@@ -1287,18 +1296,18 @@
         <v>15</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="26.1" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="12" t="s">
         <v>8</v>
@@ -1307,18 +1316,18 @@
         <v>16</v>
       </c>
       <c r="D6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="F6" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="36.950000000000003" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="12" t="s">
         <v>9</v>
@@ -1327,18 +1336,18 @@
         <v>17</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="24.95" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="12" t="s">
         <v>10</v>
@@ -1347,18 +1356,18 @@
         <v>18</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="39.950000000000003" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>11</v>
@@ -1367,18 +1376,18 @@
         <v>19</v>
       </c>
       <c r="D9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>25</v>
-      </c>
       <c r="F9" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="36.950000000000003" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="12" t="s">
         <v>12</v>
@@ -1387,18 +1396,18 @@
         <v>20</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="44.1" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="12" t="s">
         <v>13</v>
@@ -1407,20 +1416,20 @@
         <v>21</v>
       </c>
       <c r="D11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="F11" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>32</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>34</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="33" customHeight="1">
       <c r="A12" s="8"/>
       <c r="B12" s="13" t="s">
         <v>14</v>
@@ -1429,20 +1438,20 @@
         <v>22</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="4"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="18" customHeight="1">
       <c r="A13" s="8"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -1452,7 +1461,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="18" customHeight="1">
       <c r="A14" s="8"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -1462,7 +1471,7 @@
       <c r="G14" s="14"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="18" customHeight="1">
       <c r="A15" s="8"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -1472,7 +1481,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="18" customHeight="1">
       <c r="H16" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[GPR] Especificando distribuição de pontos no Product Backlog
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Product Backlog - EveRemind.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Product Backlog - EveRemind.xlsx
@@ -20,7 +20,7 @@
     <definedName name="Área_Impressão_Agenda">OFFSET(#REF!,,,COUNTA(#REF!))</definedName>
     <definedName name="Área_Impressão_Atribuição">OFFSET(#REF!,,,COUNTA(#REF!))</definedName>
     <definedName name="IníciodoCronograma">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Product Backlog'!$B$5:$G$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Product Backlog'!$B$5:$G$14</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Product Backlog'!$4:$4</definedName>
     <definedName name="TérminoAgenda">#REF!</definedName>
   </definedNames>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>NOME</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Visualizar Atividade</t>
   </si>
   <si>
-    <t>6 pontos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Uma mensagem de cadastro bem sucedido é exibida.
 </t>
   </si>
@@ -148,24 +145,204 @@
     <t>Alta</t>
   </si>
   <si>
-    <t xml:space="preserve">6 pontos
-</t>
-  </si>
-  <si>
-    <t>3 pontos</t>
-  </si>
-  <si>
-    <t>5 pontos</t>
-  </si>
-  <si>
-    <t>4 pontos</t>
+    <r>
+      <t xml:space="preserve">5 pontos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aral"/>
+      </rPr>
+      <t>2 pontos - 1 Página JSP pequena
+e 1 Página JSP média
+2 pontos - 2 Servlets
+1 ponto - Modificar DAO de Usuário</t>
+    </r>
+  </si>
+  <si>
+    <t>EST009</t>
+  </si>
+  <si>
+    <t>EST010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizar Lista
+</t>
+  </si>
+  <si>
+    <t>Visualizar Calendario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A lista de atividades pode ser vista de diferentes modos de ordenação e filtros
+</t>
+  </si>
+  <si>
+    <t>O calendário com as astividades de cada dia é mostrado para o 
+usuário</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4 pontos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aral"/>
+      </rPr>
+      <t>2 pontos - 1 Página JSP Grande
+2 pontos - 2 Servlets</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 pontos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aral"/>
+      </rPr>
+      <t>1 ponto - 1 Página JSP média
+1 ponto - 1 Servlet
+1 ponto - Modificar DAO de Atividade</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5 pontos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aral"/>
+      </rPr>
+      <t>1 ponto - 1 Página JSP média
+2 pontos - 2 Servlets
+2 pontos - Modificar DAO de Categoria
+e criar DAO de Atividade</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 pontos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aral"/>
+      </rPr>
+      <t>1 ponto - 1 Página JSP pequena
+1 ponto - 1 Servlet
+1 ponto - Modificar DAO de Categoria</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6 pontos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aral"/>
+      </rPr>
+      <t>2 pontos - 1 Página JSP grande
+2 pontos - 2 Servlets
+1 ponto - Classe Atividade
+1 ponto - DAO de Categoria</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6 pontos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aral"/>
+      </rPr>
+      <t>2 pontos - 1 Página JSP grande</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Aral"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aral"/>
+      </rPr>
+      <t>2 pontos - 2 Servlets
+1 ponto - Classes User e Hash
+1 ponto - DAO de Usuário</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 pontos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aral"/>
+      </rPr>
+      <t>1 ponto - 1 Página JSP média
+1 ponto - 1 Servlet
+1 ponto - Modificar DAO de Usuário</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8 pontos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3 pontos - Página JSP Complexa
+4 pontos - 4 Servlets
+1 ponto - Modificar DAO de Atividade</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8 pontos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4 pontos - Página JSP Complexa e
+bastante dinâmica
+4 pontos - 4 Servlets</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -208,6 +385,23 @@
       <sz val="12"/>
       <name val="Aral"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Aral"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -244,7 +438,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -293,6 +487,21 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -302,6 +511,7 @@
   <dxfs count="24">
     <dxf>
       <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -792,8 +1002,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="123825" y="781050"/>
-          <a:ext cx="2162175" cy="514350"/>
+          <a:off x="123265" y="781610"/>
+          <a:ext cx="2162735" cy="512109"/>
           <a:chOff x="114300" y="781050"/>
           <a:chExt cx="1836964" cy="514350"/>
         </a:xfrm>
@@ -933,14 +1143,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabListadeAulas" displayName="tabListadeAulas" ref="B4:G12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabListadeAulas" displayName="tabListadeAulas" ref="B4:G14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="5"/>
     <tableColumn id="2" name="NOME" dataDxfId="4"/>
-    <tableColumn id="3" name="IMPORTANCIA" dataDxfId="3"/>
-    <tableColumn id="4" name="ESTIMATIVA INICIAL" dataDxfId="2"/>
+    <tableColumn id="3" name="IMPORTANCIA" dataDxfId="2"/>
+    <tableColumn id="4" name="ESTIMATIVA INICIAL" dataDxfId="0"/>
     <tableColumn id="5" name="COMO DEMONSTRAR" dataDxfId="1"/>
-    <tableColumn id="6" name="NOTAS " dataDxfId="0"/>
+    <tableColumn id="6" name="NOTAS " dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Visão geral do semestre" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1218,8 +1428,8 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1"/>
@@ -1227,8 +1437,8 @@
     <col min="1" max="1" width="1.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="37.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="74.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="82.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
@@ -1287,7 +1497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="36" customHeight="1">
+    <row r="5" spans="1:10" ht="81.75" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="10" t="s">
         <v>7</v>
@@ -1296,18 +1506,18 @@
         <v>15</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="26.1" customHeight="1">
+    <row r="6" spans="1:10" ht="73.5" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="12" t="s">
         <v>8</v>
@@ -1316,18 +1526,18 @@
         <v>16</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="36.950000000000003" customHeight="1">
+    <row r="7" spans="1:10" ht="84.75" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="12" t="s">
         <v>9</v>
@@ -1336,18 +1546,18 @@
         <v>17</v>
       </c>
       <c r="D7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>36</v>
-      </c>
       <c r="F7" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="24.95" customHeight="1">
+    <row r="8" spans="1:10" ht="79.5" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="12" t="s">
         <v>10</v>
@@ -1356,18 +1566,18 @@
         <v>18</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>44</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="39.950000000000003" customHeight="1">
+    <row r="9" spans="1:10" ht="73.5" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>11</v>
@@ -1376,18 +1586,18 @@
         <v>19</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="36.950000000000003" customHeight="1">
+    <row r="10" spans="1:10" ht="90" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="12" t="s">
         <v>12</v>
@@ -1396,18 +1606,18 @@
         <v>20</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>42</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="44.1" customHeight="1">
+    <row r="11" spans="1:10" ht="66.75" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="12" t="s">
         <v>13</v>
@@ -1416,20 +1626,20 @@
         <v>21</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="33" customHeight="1">
+    <row r="12" spans="1:10" ht="49.5" customHeight="1">
       <c r="A12" s="8"/>
       <c r="B12" s="13" t="s">
         <v>14</v>
@@ -1438,37 +1648,59 @@
         <v>22</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="4"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="18" customHeight="1">
+    <row r="13" spans="1:10" ht="77.25" customHeight="1">
       <c r="A13" s="8"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="B13" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="18" customHeight="1">
+    <row r="14" spans="1:10" ht="69" customHeight="1">
       <c r="A14" s="8"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="B14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="13"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1">

</xml_diff>